<commit_message>
Estilizando a IDE online e desenvolvendo suas funcionalidades
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog.xlsx
+++ b/Documentação/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\projeto_individual_dashboard_e_api\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\aiello_technology_education\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D987C1-2B15-47BB-86F1-B48694B437DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EF04E0-1CC6-4889-8F3F-4F0F51B76602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Essencial</t>
   </si>
@@ -120,21 +142,9 @@
     <t>Perguntas e respostas dos Testes</t>
   </si>
   <si>
-    <t>Elaboração de Tutoriais de HTML (WebSite)</t>
-  </si>
-  <si>
-    <t>Elaboração de Tutoriais de CSS (WebSite)</t>
-  </si>
-  <si>
-    <t>Elaboração de Tutoriais de JS (WebSite)</t>
-  </si>
-  <si>
     <t>GG</t>
   </si>
   <si>
-    <t>Montagem dos Certificados</t>
-  </si>
-  <si>
     <t>BACKLOG AielloTech</t>
   </si>
   <si>
@@ -195,9 +205,6 @@
     <t>Montar ao menos um tutorial básico a respeito de JS</t>
   </si>
   <si>
-    <t>Montar os certificados que estarão disponíveis para os usuários que finalizarem os testes e alcançarem a nota mínima</t>
-  </si>
-  <si>
     <t>Montar os slides que farão parte da apresentação desse projeto</t>
   </si>
   <si>
@@ -219,17 +226,29 @@
     <t>Monstar um diagrama que mostre o funcionamento do meu projeto de maneira facilitada e intuitiva</t>
   </si>
   <si>
-    <t>Conexão da Dashboard com a API</t>
-  </si>
-  <si>
-    <t>Realizar a conexão dos dados provinientes do Arduino, cadastrados no Banco de Dados e plotarem nos gráficos em tempo real</t>
+    <t>Desenvolver o CSS e o HTML da IDE Online</t>
+  </si>
+  <si>
+    <t>Desenvolver a parte visual da sessão que será destinada a ferramenta IDE online</t>
+  </si>
+  <si>
+    <t>Estabelecer a funcionalidade a IDE Online</t>
+  </si>
+  <si>
+    <t>Elaboração de Testes de HTML (WebSite)</t>
+  </si>
+  <si>
+    <t>Elaboração de Testes de CSS (WebSite)</t>
+  </si>
+  <si>
+    <t>Elaboração de Testes de JS (WebSite)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,13 +283,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -291,18 +303,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -397,7 +409,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -413,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,34 +468,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -475,74 +504,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1101,17 +1076,20 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$C$4:$C$6</c:f>
+              <c:f>Burndown!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>87</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1210,17 +1188,20 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$D$4:$D$6</c:f>
+              <c:f>Burndown!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1264,12 +1245,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$6</c:f>
+              <c:f>Burndown!$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2156,7 +2137,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>417286</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>60778</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2186,32 +2167,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:H21" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:H21" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A2:H21" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H20">
-    <sortCondition ref="G2:G20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H21">
+    <sortCondition ref="G2:G21"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{89CF454A-6A6D-43EE-AE02-697D296142E6}" name="Descrição" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{89CF454A-6A6D-43EE-AE02-697D296142E6}" name="Descrição" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2815C1C9-FAC6-48CA-A3DE-3079D74386C9}" name="Tabela14" displayName="Tabela14" ref="B3:D6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
-  <autoFilter ref="B3:D6" xr:uid="{2815C1C9-FAC6-48CA-A3DE-3079D74386C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2815C1C9-FAC6-48CA-A3DE-3079D74386C9}" name="Tabela14" displayName="Tabela14" ref="B3:D7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+  <autoFilter ref="B3:D7" xr:uid="{2815C1C9-FAC6-48CA-A3DE-3079D74386C9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B8FE07CE-CCCC-476C-BC38-05A7E0DB61A5}" name="Sprint" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{77F17E8D-286F-4A05-98A6-08F09E6CE442}" name="Pontos Planejados" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{60195D5D-F9FF-4869-9559-32855796F538}" name="Pontos Realizados" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{B8FE07CE-CCCC-476C-BC38-05A7E0DB61A5}" name="Sprint" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{77F17E8D-286F-4A05-98A6-08F09E6CE442}" name="Pontos Planejados" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{60195D5D-F9FF-4869-9559-32855796F538}" name="Pontos Realizados" dataDxfId="6">
       <calculatedColumnFormula>SUMIF(Tabela2[[#All],[Sprint]],Tabela14[[#This Row],[Sprint]],Tabela2[[#All],[Tamanho ('#)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2485,7 +2466,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2502,7 +2483,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -2513,28 +2494,28 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2543,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -2569,7 +2550,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -2595,13 +2576,13 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6">
         <v>21</v>
@@ -2609,11 +2590,11 @@
       <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="16">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -2622,13 +2603,13 @@
         <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5">
         <v>21</v>
@@ -2640,15 +2621,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -2660,21 +2641,21 @@
         <v>13</v>
       </c>
       <c r="F7" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -2686,21 +2667,21 @@
         <v>5</v>
       </c>
       <c r="F8" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -2712,13 +2693,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
@@ -2726,7 +2707,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -2738,21 +2719,21 @@
         <v>13</v>
       </c>
       <c r="F10" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
@@ -2770,15 +2751,15 @@
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -2796,15 +2777,15 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -2822,50 +2803,50 @@
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1">
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F15" s="5">
         <v>3</v>
@@ -2874,15 +2855,15 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
@@ -2897,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>7</v>
@@ -2905,51 +2886,51 @@
     </row>
     <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="F17" s="5">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
-        <v>2</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>7</v>
@@ -2957,80 +2938,78 @@
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" s="5">
         <v>3</v>
       </c>
       <c r="G19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
+      <c r="A20" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E20" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5">
         <v>3</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E21" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5">
         <v>2</v>
       </c>
       <c r="G21" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3086,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980DA63-D86F-41BF-A596-E808F145E659}">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3106,26 +3085,26 @@
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12">
-        <f>SUM(C4:C6)</f>
+      <c r="C2" s="11">
+        <f>SUM(C4:C7)</f>
         <v>174</v>
       </c>
-      <c r="D2" s="13">
-        <f>SUM(D4:D6)</f>
-        <v>178</v>
+      <c r="D2" s="12">
+        <f>SUM(D4:D7)</f>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3134,7 +3113,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="8">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="D4" s="8">
         <f>SUMIF(Tabela2[[#All],[Sprint]],Tabela14[[#This Row],[Sprint]],Tabela2[[#All],[Tamanho ('#)]])</f>
@@ -3146,11 +3125,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="8">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="D5" s="8">
         <f>SUMIF(Tabela2[[#All],[Sprint]],Tabela14[[#This Row],[Sprint]],Tabela2[[#All],[Tamanho ('#)]])</f>
-        <v>110</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -3158,31 +3137,43 @@
         <v>3</v>
       </c>
       <c r="C6" s="8">
+        <v>58</v>
+      </c>
+      <c r="D6" s="21">
+        <f>SUMIF(Tabela2[[#All],[Sprint]],Tabela14[[#This Row],[Sprint]],Tabela2[[#All],[Tamanho ('#)]])</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="8">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9">
-        <f>SUM(Tabela2[Tamanho ('#)])/2</f>
-        <v>89</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="C9" s="23" cm="1">
+        <f t="array" ref="C9">SUM(Tabela2[Tamanho ('#)]/3)</f>
+        <v>58.333333333333329</v>
+      </c>
+      <c r="D9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="D6" calculatedColumn="1"/>
+    <ignoredError sqref="D7" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Upload da documentação do projeto e alterações nos slides e no backlog
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog.xlsx
+++ b/Documentação/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\aiello_technology_education\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EF04E0-1CC6-4889-8F3F-4F0F51B76602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD2389F-EAB1-488C-88B4-343E0CCA69AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Essencial</t>
   </si>
@@ -76,21 +76,12 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
     <t>Finalizada</t>
   </si>
   <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
-    <t>Desejável</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>Diagrama de Solução</t>
   </si>
   <si>
-    <t>Diagrama de Negócio</t>
-  </si>
-  <si>
     <t>Criar um repositório no GitHub para armazenar todos os arquivos e diretórios que fazem parte do projeto</t>
   </si>
   <si>
@@ -221,9 +209,6 @@
   </si>
   <si>
     <t>Montar um diagrama que mostre a arquitetura técnica que estou utilizando para esse projeto</t>
-  </si>
-  <si>
-    <t>Monstar um diagrama que mostre o funcionamento do meu projeto de maneira facilitada e intuitiva</t>
   </si>
   <si>
     <t>Desenvolver o CSS e o HTML da IDE Online</t>
@@ -442,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -492,26 +477,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,7 +1175,7 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2167,10 +2143,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:H21" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A2:H21" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H21">
-    <sortCondition ref="G2:G21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:H20" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A2:H20" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H20">
+    <sortCondition ref="G2:G20"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="20"/>
@@ -2463,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2482,20 +2458,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -2504,19 +2480,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
@@ -2524,13 +2500,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5">
         <v>3</v>
@@ -2542,21 +2518,21 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
@@ -2568,21 +2544,21 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6">
         <v>21</v>
@@ -2594,22 +2570,22 @@
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5">
         <v>21</v>
@@ -2621,21 +2597,21 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5">
         <v>13</v>
@@ -2647,21 +2623,21 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5">
         <v>5</v>
@@ -2678,16 +2654,16 @@
     </row>
     <row r="9" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5">
         <v>8</v>
@@ -2699,21 +2675,21 @@
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5">
         <v>13</v>
@@ -2725,21 +2701,21 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="5">
         <v>8</v>
@@ -2751,21 +2727,21 @@
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5">
         <v>8</v>
@@ -2777,21 +2753,21 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5">
         <v>13</v>
@@ -2803,21 +2779,21 @@
         <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5">
         <v>5</v>
@@ -2829,21 +2805,21 @@
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -2855,21 +2831,21 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" s="5">
         <v>5</v>
@@ -2881,21 +2857,21 @@
         <v>3</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E17" s="5">
         <v>13</v>
@@ -2907,21 +2883,21 @@
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E18" s="5">
         <v>8</v>
@@ -2933,48 +2909,48 @@
         <v>3</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="5">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="5">
-        <v>3</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="20" t="s">
+    <row r="20" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F20" s="5">
         <v>2</v>
@@ -2983,32 +2959,6 @@
         <v>3</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="5">
-        <v>5</v>
-      </c>
-      <c r="F21" s="5">
-        <v>2</v>
-      </c>
-      <c r="G21" s="5">
-        <v>3</v>
-      </c>
-      <c r="H21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3016,7 +2966,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:F21 H3:H21">
+  <conditionalFormatting sqref="C3:F20 H3:H20">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
@@ -3027,7 +2977,7 @@
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H21">
+  <conditionalFormatting sqref="H3:H20">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -3039,19 +2989,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:G21" xr:uid="{E9CF9112-A7D5-4A3C-8BE7-64942B77F025}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:G20" xr:uid="{E9CF9112-A7D5-4A3C-8BE7-64942B77F025}">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C21" xr:uid="{8630AD09-0144-4519-A158-ED3BE3A9872A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C20" xr:uid="{8630AD09-0144-4519-A158-ED3BE3A9872A}">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H21" xr:uid="{C0662D32-9D3B-4AF6-A8DD-256816F071DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H20" xr:uid="{C0662D32-9D3B-4AF6-A8DD-256816F071DB}">
       <formula1>"Pendente,Em Andamento, Finalizada"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D21" xr:uid="{14DF18D5-D0D6-460C-9DD3-F79140E2407B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D20" xr:uid="{14DF18D5-D0D6-460C-9DD3-F79140E2407B}">
       <formula1>"PP,P,M,G,GG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E21" xr:uid="{007AAA73-0A84-4DF3-8313-6B93A73F8B5E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E20" xr:uid="{007AAA73-0A84-4DF3-8313-6B93A73F8B5E}">
       <formula1>"3,5,8,13,21"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3086,7 +3036,7 @@
     </row>
     <row r="2" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="11">
         <f>SUM(C4:C7)</f>
@@ -3094,7 +3044,7 @@
       </c>
       <c r="D2" s="12">
         <f>SUM(D4:D7)</f>
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -3102,10 +3052,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -3139,9 +3089,9 @@
       <c r="C6" s="8">
         <v>58</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="8">
         <f>SUMIF(Tabela2[[#All],[Sprint]],Tabela14[[#This Row],[Sprint]],Tabela2[[#All],[Tamanho ('#)]])</f>
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -3161,12 +3111,12 @@
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="23" cm="1">
+      <c r="B9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="18" cm="1">
         <f t="array" ref="C9">SUM(Tabela2[Tamanho ('#)]/3)</f>
-        <v>58.333333333333329</v>
+        <v>56.666666666666664</v>
       </c>
       <c r="D9" s="8"/>
     </row>

</xml_diff>